<commit_message>
Correção dos eventos 7, 8, 9 e adicionada uma observação-dúvida sobre o evento 10 para o professor checar
</commit_message>
<xml_diff>
--- a/17- Análise de Eventos para cada Cenário.xlsx
+++ b/17- Análise de Eventos para cada Cenário.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bixdi\Desktop\salada de pepino\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Capacidade</t>
   </si>
@@ -108,20 +113,29 @@
     <t>x(6)</t>
   </si>
   <si>
-    <t>Finalização da venda</t>
-  </si>
-  <si>
     <t>EXTERNO</t>
   </si>
   <si>
     <t>TEMPORAL</t>
+  </si>
+  <si>
+    <t>Finalização do pedido</t>
+  </si>
+  <si>
+    <t>OBS: Estamos na dúvida se o evento 10</t>
+  </si>
+  <si>
+    <t>poderia entrar como um não-evento</t>
+  </si>
+  <si>
+    <t>de falha, ao invés de entrar em FA.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +189,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -292,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -303,76 +323,86 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -419,7 +449,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,9 +481,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -485,6 +516,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -660,14 +692,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
@@ -676,18 +708,19 @@
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="E1" s="27" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-    </row>
-    <row r="2" spans="1:10" ht="30.75" thickBot="1">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,227 +750,245 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="11"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="12">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="11"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="12">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="9">
         <v>3</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="11"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="12">
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="9">
         <v>4</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="11"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="12">
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="9">
         <v>5</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="11"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="12">
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="9">
         <v>6</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18">
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="14">
         <v>7</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22" t="s">
+      <c r="D9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="11"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
       <c r="B10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>8</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="9">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="28">
+        <v>10</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="9">
+        <v>11</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="9">
+        <v>12</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="11"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="12">
-        <v>9</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="11"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="12">
-        <v>10</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="11"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="12">
-        <v>11</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="26"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="12">
-        <v>12</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="27" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -952,24 +1003,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>